<commit_message>
Automatizacino mi formato y cambios en UsuarioNorm
</commit_message>
<xml_diff>
--- a/RegistraUSNormales.xlsx
+++ b/RegistraUSNormales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\VisualProg\PRUBAS Funcionales RESI\EXELS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA95FE4-CBD9-445B-9BEC-EA8EABA53724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B30A842-A4DD-47A7-9D26-CAD2B9D40EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14280" yWindow="195" windowWidth="14775" windowHeight="7305" xr2:uid="{947B47C3-8618-4FEC-A9ED-74542C012D18}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{947B47C3-8618-4FEC-A9ED-74542C012D18}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
   <si>
     <t>Academia</t>
   </si>
@@ -78,18 +78,6 @@
     <t xml:space="preserve">Ingeniería en Sistemas Computacionales </t>
   </si>
   <si>
-    <t>Ingeniería en Electromecánica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingeniería Industrial </t>
-  </si>
-  <si>
-    <t>Ingeniería en Gestión Empresarial</t>
-  </si>
-  <si>
-    <t>Contador Publico</t>
-  </si>
-  <si>
     <t>alumno230007</t>
   </si>
   <si>
@@ -148,6 +136,21 @@
   </si>
   <si>
     <t>NombreDelEstuduante</t>
+  </si>
+  <si>
+    <t>Numerocontrolgrupo</t>
+  </si>
+  <si>
+    <t>grup0012023</t>
+  </si>
+  <si>
+    <t>grup0022023</t>
+  </si>
+  <si>
+    <t>grup0032023</t>
+  </si>
+  <si>
+    <t>grup0042023</t>
   </si>
 </sst>
 </file>
@@ -199,8 +202,8 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -516,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AFA5109-4B52-4F7B-A729-6A6FE5ACD800}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,18 +533,21 @@
     <col min="4" max="4" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -551,8 +557,11 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -562,8 +571,11 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -573,10 +585,13 @@
       <c r="C4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -584,10 +599,13 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -595,10 +613,13 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -606,108 +627,139 @@
       <c r="C7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="D7" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="D12" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C13" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="D13" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>20</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C14" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="D14" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
         <v>21</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C15" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="D15" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
         <v>22</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
+      <c r="D16" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>